<commit_message>
Add column that repeats for testing multiple measurements of the same attribute
</commit_message>
<xml_diff>
--- a/test_data/double.xlsx
+++ b/test_data/double.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -87,6 +87,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,12 +137,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,7 +172,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -206,6 +216,9 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="ALT1" s="0"/>
@@ -247,7 +260,10 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>114.152610788288</v>
+        <v>127.768450534542</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>105.1013</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,6 +290,9 @@
       </c>
       <c r="I3" s="0" t="n">
         <v>120.987</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>120.986</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Implement multiple file support
</commit_message>
<xml_diff>
--- a/test_data/double.xlsx
+++ b/test_data/double.xlsx
@@ -49,13 +49,13 @@
     <t xml:space="preserve">S:bead width (mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">S1</t>
+    <t xml:space="preserve">DOUBLES1</t>
   </si>
   <si>
     <t xml:space="preserve">Ti-6Al-4V</t>
   </si>
   <si>
-    <t xml:space="preserve">S5</t>
+    <t xml:space="preserve">DOUBLES5</t>
   </si>
 </sst>
 </file>
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -87,12 +87,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,16 +131,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,7 +162,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,7 +208,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="ALT1" s="0"/>
@@ -260,7 +250,7 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>127.768450534542</v>
+        <v>116.988752455735</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>105.1013</v>

</xml_diff>